<commit_message>
se agregaron más datos
</commit_message>
<xml_diff>
--- a/ranking-10-Vinos.xlsx
+++ b/ranking-10-Vinos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
   <si>
     <t>Posición</t>
   </si>
@@ -41,10 +41,40 @@
     <t>Varietal</t>
   </si>
   <si>
+    <t>Vino El Cóndor</t>
+  </si>
+  <si>
+    <t>7.1</t>
+  </si>
+  <si>
+    <t>5500.0</t>
+  </si>
+  <si>
+    <t>Bodega Lopez</t>
+  </si>
+  <si>
+    <t>Zona Centro-Oeste</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Cabernet</t>
+  </si>
+  <si>
+    <t>Gran Vino Mendoza</t>
+  </si>
+  <si>
+    <t>4.7</t>
+  </si>
+  <si>
+    <t>3500.0</t>
+  </si>
+  <si>
     <t>Vino Regional 2019</t>
   </si>
   <si>
-    <t>9.3</t>
+    <t>4.3</t>
   </si>
   <si>
     <t>2000.0</t>
@@ -56,88 +86,64 @@
     <t>Zona Noreste</t>
   </si>
   <si>
-    <t>Argentina</t>
-  </si>
-  <si>
     <t>Malbec</t>
   </si>
   <si>
+    <t>Gran Reserva 2015</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>2500.0</t>
+  </si>
+  <si>
     <t>Vino Nacional</t>
   </si>
   <si>
-    <t>9.1</t>
+    <t>4.1</t>
   </si>
   <si>
     <t>1500.0</t>
   </si>
   <si>
-    <t>Bodega Lopez</t>
-  </si>
-  <si>
-    <t>Zona Centro-Oeste</t>
+    <t>San Juan Reserva</t>
+  </si>
+  <si>
+    <t>3000.0</t>
+  </si>
+  <si>
+    <t>Tinto Gaucho</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>1700.0</t>
   </si>
   <si>
     <t>Merlot Clásico</t>
   </si>
   <si>
+    <t>3.1</t>
+  </si>
+  <si>
     <t>1300.0</t>
   </si>
   <si>
-    <t>Cabernet</t>
-  </si>
-  <si>
     <t>Vino de La Rioja</t>
   </si>
   <si>
-    <t>9.0</t>
+    <t>3.0</t>
   </si>
   <si>
     <t>6000.0</t>
   </si>
   <si>
-    <t>Tinto Gaucho</t>
-  </si>
-  <si>
-    <t>8.5</t>
-  </si>
-  <si>
-    <t>1700.0</t>
-  </si>
-  <si>
-    <t>San Juan Reserva</t>
-  </si>
-  <si>
-    <t>7.1</t>
-  </si>
-  <si>
-    <t>3000.0</t>
-  </si>
-  <si>
-    <t>Vino El Cóndor</t>
-  </si>
-  <si>
-    <t>5500.0</t>
-  </si>
-  <si>
-    <t>Gran Reserva 2015</t>
-  </si>
-  <si>
-    <t>6.7</t>
-  </si>
-  <si>
-    <t>2500.0</t>
-  </si>
-  <si>
-    <t>Gran Vino Mendoza</t>
-  </si>
-  <si>
-    <t>3500.0</t>
-  </si>
-  <si>
     <t>Vino Numero 8</t>
   </si>
   <si>
-    <t>6.1</t>
+    <t>2.7</t>
   </si>
 </sst>
 </file>
@@ -274,10 +280,10 @@
         <v>18</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s" s="0">
         <v>14</v>
@@ -291,28 +297,28 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C4" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="C4" t="n" s="0">
-        <v>7.0</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s" s="0">
+      <c r="F4" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="F4" t="s" s="0">
-        <v>12</v>
-      </c>
       <c r="G4" t="s" s="0">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="H4" t="s" s="0">
         <v>14</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
@@ -320,16 +326,16 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" t="n" s="0">
         <v>7.0</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s" s="0">
         <v>12</v>
@@ -341,7 +347,7 @@
         <v>14</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6">
@@ -349,16 +355,16 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" t="n" s="0">
         <v>7.0</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s" s="0">
         <v>12</v>
@@ -370,7 +376,7 @@
         <v>14</v>
       </c>
       <c r="I6" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7">
@@ -378,28 +384,28 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" t="n" s="0">
         <v>7.0</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s" s="0">
         <v>32</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s" s="0">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="H7" t="s" s="0">
         <v>14</v>
       </c>
       <c r="I7" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
@@ -413,22 +419,22 @@
         <v>7.0</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G8" t="s" s="0">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H8" t="s" s="0">
         <v>14</v>
       </c>
       <c r="I8" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
@@ -436,22 +442,22 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C9" t="n" s="0">
         <v>7.0</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G9" t="s" s="0">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H9" t="s" s="0">
         <v>14</v>
@@ -465,28 +471,28 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C10" t="n" s="0">
         <v>7.0</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G10" t="s" s="0">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H10" t="s" s="0">
         <v>14</v>
       </c>
       <c r="I10" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11">
@@ -494,28 +500,28 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C11" t="n" s="0">
         <v>7.0</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F11" t="s" s="0">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G11" t="s" s="0">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="H11" t="s" s="0">
         <v>14</v>
       </c>
       <c r="I11" t="s" s="0">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aplicando el patrón strategy
</commit_message>
<xml_diff>
--- a/ranking-10-Vinos.xlsx
+++ b/ranking-10-Vinos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="43">
   <si>
     <t>Posición</t>
   </si>
@@ -41,76 +41,73 @@
     <t>Varietal</t>
   </si>
   <si>
+    <t>Gran Vino Mendoza</t>
+  </si>
+  <si>
+    <t>4.7</t>
+  </si>
+  <si>
+    <t>3500.0</t>
+  </si>
+  <si>
+    <t>Bodega Lopez</t>
+  </si>
+  <si>
+    <t>Zona Centro-Oeste</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Cabernet</t>
+  </si>
+  <si>
+    <t>Vino Regional 2019</t>
+  </si>
+  <si>
+    <t>4.3</t>
+  </si>
+  <si>
+    <t>2000.0</t>
+  </si>
+  <si>
+    <t>Bodega Regional</t>
+  </si>
+  <si>
+    <t>Zona Noreste</t>
+  </si>
+  <si>
+    <t>Malbec</t>
+  </si>
+  <si>
+    <t>Gran Reserva 2015</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>2500.0</t>
+  </si>
+  <si>
+    <t>Vino Nacional</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>1500.0</t>
+  </si>
+  <si>
+    <t>San Juan Reserva</t>
+  </si>
+  <si>
+    <t>3000.0</t>
+  </si>
+  <si>
     <t>Vino El Cóndor</t>
   </si>
   <si>
-    <t>7.1</t>
-  </si>
-  <si>
     <t>5500.0</t>
-  </si>
-  <si>
-    <t>Bodega Lopez</t>
-  </si>
-  <si>
-    <t>Zona Centro-Oeste</t>
-  </si>
-  <si>
-    <t>Argentina</t>
-  </si>
-  <si>
-    <t>Cabernet</t>
-  </si>
-  <si>
-    <t>Gran Vino Mendoza</t>
-  </si>
-  <si>
-    <t>4.7</t>
-  </si>
-  <si>
-    <t>3500.0</t>
-  </si>
-  <si>
-    <t>Vino Regional 2019</t>
-  </si>
-  <si>
-    <t>4.3</t>
-  </si>
-  <si>
-    <t>2000.0</t>
-  </si>
-  <si>
-    <t>Bodega Regional</t>
-  </si>
-  <si>
-    <t>Zona Noreste</t>
-  </si>
-  <si>
-    <t>Malbec</t>
-  </si>
-  <si>
-    <t>Gran Reserva 2015</t>
-  </si>
-  <si>
-    <t>4.2</t>
-  </si>
-  <si>
-    <t>2500.0</t>
-  </si>
-  <si>
-    <t>Vino Nacional</t>
-  </si>
-  <si>
-    <t>4.1</t>
-  </si>
-  <si>
-    <t>1500.0</t>
-  </si>
-  <si>
-    <t>San Juan Reserva</t>
-  </si>
-  <si>
-    <t>3000.0</t>
   </si>
   <si>
     <t>Tinto Gaucho</t>
@@ -280,16 +277,16 @@
         <v>18</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H3" t="s" s="0">
         <v>14</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4">
@@ -297,28 +294,28 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C4" t="n" s="0">
         <v>7.0</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s" s="0">
         <v>21</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="G4" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="I4" t="s" s="0">
-        <v>24</v>
       </c>
     </row>
     <row r="5">
@@ -347,7 +344,7 @@
         <v>14</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6">
@@ -361,10 +358,10 @@
         <v>7.0</v>
       </c>
       <c r="D6" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s" s="0">
         <v>29</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>30</v>
       </c>
       <c r="F6" t="s" s="0">
         <v>12</v>
@@ -376,7 +373,7 @@
         <v>14</v>
       </c>
       <c r="I6" t="s" s="0">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
@@ -384,16 +381,16 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="C7" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s" s="0">
         <v>31</v>
-      </c>
-      <c r="C7" t="n" s="0">
-        <v>7.0</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>32</v>
       </c>
       <c r="F7" t="s" s="0">
         <v>12</v>
@@ -413,22 +410,22 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="C8" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="D8" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="C8" t="n" s="0">
-        <v>7.0</v>
-      </c>
-      <c r="D8" t="s" s="0">
+      <c r="E8" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="E8" t="s" s="0">
-        <v>35</v>
-      </c>
       <c r="F8" t="s" s="0">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G8" t="s" s="0">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H8" t="s" s="0">
         <v>14</v>
@@ -442,22 +439,22 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="C9" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="D9" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="C9" t="n" s="0">
-        <v>7.0</v>
-      </c>
-      <c r="D9" t="s" s="0">
+      <c r="E9" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="E9" t="s" s="0">
-        <v>38</v>
-      </c>
       <c r="F9" t="s" s="0">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G9" t="s" s="0">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H9" t="s" s="0">
         <v>14</v>
@@ -471,28 +468,28 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="C10" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="D10" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="C10" t="n" s="0">
-        <v>7.0</v>
-      </c>
-      <c r="D10" t="s" s="0">
+      <c r="E10" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="E10" t="s" s="0">
-        <v>41</v>
-      </c>
       <c r="F10" t="s" s="0">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G10" t="s" s="0">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H10" t="s" s="0">
         <v>14</v>
       </c>
       <c r="I10" t="s" s="0">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11">
@@ -500,16 +497,16 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="C11" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="D11" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="C11" t="n" s="0">
-        <v>7.0</v>
-      </c>
-      <c r="D11" t="s" s="0">
-        <v>43</v>
-      </c>
       <c r="E11" t="s" s="0">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F11" t="s" s="0">
         <v>12</v>
@@ -521,7 +518,7 @@
         <v>14</v>
       </c>
       <c r="I11" t="s" s="0">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>